<commit_message>
Some minor files update
</commit_message>
<xml_diff>
--- a/TGSB Case Study 1/Timesheet_01_2024.xlsx
+++ b/TGSB Case Study 1/Timesheet_01_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27923"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://totalworkplace.sharepoint.com/sites/TGSB-DemoTeam/Documents partages/General/2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/998c3e7283d5563b/00-Programing/AdvancedExcel/TGSB Case Study 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{C1AF690E-F9BE-4E83-9AC9-7E15B5B280FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D254FD55-D597-4050-AFB3-FEEE136C8B60}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="8_{C1AF690E-F9BE-4E83-9AC9-7E15B5B280FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B53356F-6E35-4BDC-B1FE-05D0A691BFCC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
@@ -40,13 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="103">
-  <si>
-    <t>SC TotalEnergies Global Services Bucharest SRL</t>
-  </si>
-  <si>
-    <t>RO37214798 J40/3436/2017</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="102">
   <si>
     <t>DEPARTMENT: All teams</t>
   </si>
@@ -349,13 +343,16 @@
   </si>
   <si>
     <t>J0000022</t>
+  </si>
+  <si>
+    <t>Company name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -546,13 +543,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,11 +856,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AL36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
@@ -876,75 +873,73 @@
     <col min="9" max="38" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:38" ht="16.5" customHeight="1"/>
-    <row r="2" spans="2:38">
-      <c r="B2" s="21" t="s">
+    <row r="1" spans="2:38" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
-    <row r="3" spans="2:38">
-      <c r="B3" s="21" t="s">
+    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
-    <row r="4" spans="2:38">
-      <c r="B4" s="21" t="s">
+    <row r="6" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="8" spans="2:38" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="H9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
     </row>
-    <row r="5" spans="2:38">
-      <c r="B5" s="21" t="s">
+    <row r="10" spans="2:38" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="H11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
     </row>
-    <row r="6" spans="2:38" ht="15" customHeight="1">
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="8" spans="2:38"/>
-    <row r="9" spans="2:38">
-      <c r="H9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="21"/>
-    </row>
-    <row r="10" spans="2:38"/>
-    <row r="11" spans="2:38">
-      <c r="H11" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="2:38"/>
-    <row r="13" spans="2:38" ht="15" customHeight="1">
+    <row r="12" spans="2:38" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -983,170 +978,170 @@
       <c r="AK13" s="18"/>
       <c r="AL13" s="18"/>
     </row>
-    <row r="14" spans="2:38" ht="128.1" customHeight="1">
+    <row r="14" spans="2:38" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="13" t="s">
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="J14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="K14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="M14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="N14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="O14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="P14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="T14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="1" t="s">
+      <c r="U14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="T14" s="3" t="s">
+      <c r="V14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U14" s="3" t="s">
+      <c r="W14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="Z14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Y14" s="1" t="s">
+      <c r="AA14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Z14" s="1" t="s">
+      <c r="AB14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AA14" s="3" t="s">
+      <c r="AC14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AB14" s="3" t="s">
+      <c r="AD14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AC14" s="1" t="s">
+      <c r="AE14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AD14" s="1" t="s">
+      <c r="AF14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AG14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AF14" s="1" t="s">
+      <c r="AH14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AG14" s="1" t="s">
+      <c r="AI14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AH14" s="3" t="s">
+      <c r="AJ14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AI14" s="3" t="s">
+      <c r="AK14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AJ14" s="1" t="s">
+      <c r="AL14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AK14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL14" s="1" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="15" spans="2:38" ht="15" customHeight="1">
+    <row r="15" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>2</v>
       </c>
       <c r="C15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="F15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="G15" s="17" t="s">
         <v>45</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
       <c r="V15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W15" s="4">
         <v>8</v>
@@ -1155,15 +1150,15 @@
         <v>8</v>
       </c>
       <c r="Y15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
       <c r="AC15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AD15" s="4">
         <v>8</v>
@@ -1175,46 +1170,46 @@
         <v>8</v>
       </c>
       <c r="AG15" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH15" s="7"/>
       <c r="AI15" s="7"/>
       <c r="AJ15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL15" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>8</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AK15" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AL15" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="2:38" ht="15" customHeight="1">
-      <c r="B16" s="4">
-        <v>8</v>
-      </c>
-      <c r="C16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="F16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="G16" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L16" s="4">
         <v>8</v>
@@ -1225,13 +1220,13 @@
         <v>8</v>
       </c>
       <c r="P16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S16" s="4">
         <v>8</v>
@@ -1242,13 +1237,13 @@
         <v>8</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z16" s="4">
         <v>8</v>
@@ -1256,14 +1251,14 @@
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
       <c r="AC16" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD16" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE16" s="5"/>
       <c r="AF16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AG16" s="4">
         <v>8</v>
@@ -1274,46 +1269,46 @@
         <v>8</v>
       </c>
       <c r="AK16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:38" ht="15" customHeight="1">
+    <row r="17" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>13</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K17" s="4">
         <v>8</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P17" s="4">
         <v>8</v>
@@ -1322,10 +1317,10 @@
         <v>8</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
@@ -1336,13 +1331,13 @@
         <v>8</v>
       </c>
       <c r="X17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
@@ -1354,41 +1349,41 @@
       </c>
       <c r="AE17" s="5"/>
       <c r="AF17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AG17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK17" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL17" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:38" ht="15" customHeight="1">
+    <row r="18" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>22</v>
       </c>
       <c r="C18" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="F18" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="G18" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="10">
@@ -1398,18 +1393,18 @@
         <v>10.3</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
       <c r="O18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q18" s="4">
         <v>11</v>
@@ -1418,7 +1413,7 @@
         <v>8</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
@@ -1430,10 +1425,10 @@
         <v>8</v>
       </c>
       <c r="Y18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
@@ -1445,15 +1440,15 @@
       </c>
       <c r="AE18" s="5"/>
       <c r="AF18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AG18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH18" s="7"/>
       <c r="AI18" s="7"/>
       <c r="AJ18" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK18" s="4">
         <v>8</v>
@@ -1462,52 +1457,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:38" ht="15" customHeight="1">
+    <row r="19" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>18</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
       <c r="O19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P19" s="4">
         <v>8</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T19" s="7"/>
       <c r="U19" s="7"/>
@@ -1515,83 +1510,83 @@
         <v>8</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
       <c r="AC19" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD19" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE19" s="5"/>
       <c r="AF19" s="4">
         <v>8</v>
       </c>
       <c r="AG19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH19" s="7"/>
       <c r="AI19" s="7"/>
       <c r="AJ19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL19" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:38" ht="15" customHeight="1">
+    <row r="20" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>5</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="10">
         <v>11</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
       <c r="O20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q20" s="4">
         <v>8</v>
@@ -1600,15 +1595,15 @@
         <v>8</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
       <c r="V20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X20" s="4">
         <v>8</v>
@@ -1617,7 +1612,7 @@
         <v>8</v>
       </c>
       <c r="Z20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
@@ -1625,52 +1620,52 @@
         <v>8</v>
       </c>
       <c r="AD20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AE20" s="10">
         <v>9</v>
       </c>
       <c r="AF20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AG20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
       <c r="AJ20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL20" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:38" ht="15" customHeight="1">
+    <row r="21" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>6</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K21" s="4">
         <v>8</v>
@@ -1681,7 +1676,7 @@
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
       <c r="O21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P21" s="4">
         <v>8</v>
@@ -1693,12 +1688,12 @@
         <v>8</v>
       </c>
       <c r="S21" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
       <c r="V21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W21" s="4">
         <v>8</v>
@@ -1707,18 +1702,18 @@
         <v>8</v>
       </c>
       <c r="Y21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA21" s="7"/>
       <c r="AB21" s="7"/>
       <c r="AC21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AD21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AE21" s="5"/>
       <c r="AF21" s="4">
@@ -1730,7 +1725,7 @@
       <c r="AH21" s="7"/>
       <c r="AI21" s="7"/>
       <c r="AJ21" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK21" s="4">
         <v>8</v>
@@ -1739,52 +1734,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:38" ht="15" customHeight="1">
+    <row r="22" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>20</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K22" s="4">
         <v>8</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P22" s="4">
         <v>8</v>
       </c>
       <c r="Q22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R22" s="4">
         <v>8</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
@@ -1795,21 +1790,21 @@
         <v>8</v>
       </c>
       <c r="X22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z22" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA22" s="7"/>
       <c r="AB22" s="7"/>
       <c r="AC22" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AE22" s="10">
         <v>9</v>
@@ -1818,7 +1813,7 @@
         <v>8</v>
       </c>
       <c r="AG22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="7"/>
@@ -1826,30 +1821,30 @@
         <v>8</v>
       </c>
       <c r="AK22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL22" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="23" spans="2:38" ht="15" customHeight="1">
+    <row r="23" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>17</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E23" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="10">
@@ -1859,15 +1854,15 @@
         <v>9</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
       <c r="O23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P23" s="4">
         <v>8</v>
@@ -1876,18 +1871,18 @@
         <v>8</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
       <c r="V23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X23" s="4">
         <v>8</v>
@@ -1896,51 +1891,51 @@
         <v>8</v>
       </c>
       <c r="Z23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA23" s="7"/>
       <c r="AB23" s="7"/>
       <c r="AC23" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD23" s="11"/>
       <c r="AE23" s="5"/>
       <c r="AF23" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG23" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH23" s="7"/>
       <c r="AI23" s="7"/>
       <c r="AJ23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK23" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL23" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:38" ht="15" customHeight="1">
+    <row r="24" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>10</v>
       </c>
       <c r="C24" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="F24" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="G24" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1968,7 +1963,7 @@
         <v>8</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
@@ -2014,31 +2009,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:38" ht="15" customHeight="1">
+    <row r="25" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>15</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E25" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="10">
         <v>9</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K25" s="4">
         <v>8</v>
@@ -2049,19 +2044,19 @@
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
@@ -2072,18 +2067,18 @@
         <v>8</v>
       </c>
       <c r="X25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA25" s="7"/>
       <c r="AB25" s="7"/>
       <c r="AC25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AD25" s="4">
         <v>8</v>
@@ -2092,7 +2087,7 @@
         <v>9</v>
       </c>
       <c r="AF25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AG25" s="4">
         <v>8</v>
@@ -2100,7 +2095,7 @@
       <c r="AH25" s="7"/>
       <c r="AI25" s="7"/>
       <c r="AJ25" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK25" s="4">
         <v>8</v>
@@ -2109,32 +2104,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:38" ht="15" customHeight="1">
+    <row r="26" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>4</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E26" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L26" s="4">
         <v>8</v>
@@ -2148,35 +2143,35 @@
         <v>8</v>
       </c>
       <c r="Q26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
       <c r="V26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W26" s="4">
         <v>8</v>
       </c>
       <c r="X26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y26" s="4">
         <v>8</v>
       </c>
       <c r="Z26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA26" s="7"/>
       <c r="AB26" s="7"/>
       <c r="AC26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AD26" s="4">
         <v>8</v>
@@ -2185,15 +2180,15 @@
         <v>9</v>
       </c>
       <c r="AF26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AG26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH26" s="7"/>
       <c r="AI26" s="7"/>
       <c r="AJ26" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK26" s="4">
         <v>8</v>
@@ -2202,24 +2197,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:38" ht="15" customHeight="1">
+    <row r="27" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>9</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -2227,27 +2222,27 @@
         <v>8</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P27" s="4">
         <v>8</v>
       </c>
       <c r="Q27" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R27" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S27" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
@@ -2255,7 +2250,7 @@
         <v>8</v>
       </c>
       <c r="W27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X27" s="4">
         <v>8</v>
@@ -2264,12 +2259,12 @@
         <v>8</v>
       </c>
       <c r="Z27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA27" s="7"/>
       <c r="AB27" s="7"/>
       <c r="AC27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AD27" s="4">
         <v>8</v>
@@ -2279,38 +2274,38 @@
         <v>8</v>
       </c>
       <c r="AG27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH27" s="7"/>
       <c r="AI27" s="7"/>
       <c r="AJ27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK27" s="4">
         <v>8</v>
       </c>
       <c r="AL27" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="28" spans="2:38" ht="15" customHeight="1">
+    <row r="28" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>21</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E28" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -2318,10 +2313,10 @@
         <v>8</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
@@ -2332,13 +2327,13 @@
         <v>8</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
@@ -2349,18 +2344,18 @@
         <v>8</v>
       </c>
       <c r="X28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA28" s="7"/>
       <c r="AB28" s="7"/>
       <c r="AC28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AD28" s="4">
         <v>8</v>
@@ -2370,7 +2365,7 @@
         <v>8</v>
       </c>
       <c r="AG28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH28" s="7"/>
       <c r="AI28" s="7"/>
@@ -2381,52 +2376,52 @@
         <v>8</v>
       </c>
       <c r="AL28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="29" spans="2:38" ht="15" customHeight="1">
+    <row r="29" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>16</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E29" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q29" s="4">
         <v>8</v>
       </c>
       <c r="R29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S29" s="4">
         <v>8</v>
@@ -2434,10 +2429,10 @@
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
       <c r="V29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X29" s="4">
         <v>8</v>
@@ -2446,15 +2441,15 @@
         <v>8</v>
       </c>
       <c r="Z29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
       <c r="AC29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AD29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AE29" s="10">
         <v>9</v>
@@ -2463,12 +2458,12 @@
         <v>8</v>
       </c>
       <c r="AG29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH29" s="7"/>
       <c r="AI29" s="7"/>
       <c r="AJ29" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK29" s="4">
         <v>8</v>
@@ -2477,34 +2472,34 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="2:38" ht="15" customHeight="1">
+    <row r="30" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>3</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E30" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="10">
         <v>9</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L30" s="4">
         <v>8</v>
@@ -2518,13 +2513,13 @@
         <v>8</v>
       </c>
       <c r="Q30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T30" s="7"/>
       <c r="U30" s="7"/>
@@ -2535,13 +2530,13 @@
         <v>8</v>
       </c>
       <c r="X30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
@@ -2555,10 +2550,10 @@
         <v>9</v>
       </c>
       <c r="AF30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AG30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH30" s="7"/>
       <c r="AI30" s="7"/>
@@ -2566,69 +2561,69 @@
         <v>8</v>
       </c>
       <c r="AK30" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL30" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:38" ht="15" customHeight="1">
+    <row r="31" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>12</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E31" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
       <c r="V31" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W31" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X31" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y31" s="4">
         <v>8</v>
@@ -2662,40 +2657,40 @@
         <v>8</v>
       </c>
       <c r="AL31" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="32" spans="2:38" ht="15" customHeight="1">
+    <row r="32" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>11</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E32" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="10">
         <v>9</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K32" s="4">
         <v>8</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
@@ -2706,10 +2701,10 @@
         <v>8</v>
       </c>
       <c r="Q32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S32" s="4">
         <v>8</v>
@@ -2723,13 +2718,13 @@
         <v>8</v>
       </c>
       <c r="X32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA32" s="7"/>
       <c r="AB32" s="7"/>
@@ -2737,7 +2732,7 @@
         <v>8</v>
       </c>
       <c r="AD32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AE32" s="10">
         <v>9</v>
@@ -2746,7 +2741,7 @@
         <v>8</v>
       </c>
       <c r="AG32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH32" s="7"/>
       <c r="AI32" s="7"/>
@@ -2757,136 +2752,136 @@
         <v>8</v>
       </c>
       <c r="AL32" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="33" spans="2:38" ht="15" customHeight="1">
+    <row r="33" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>1</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E33" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G33" s="17" t="s">
         <v>60</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>62</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="V33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="W33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="X33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Y33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Z33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AA33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AB33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AC33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AD33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AE33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AF33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AG33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AH33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AI33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AJ33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AK33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="AL33" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:38" ht="15" customHeight="1">
+    <row r="34" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>7</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E34" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -2897,12 +2892,12 @@
         <v>8</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P34" s="4">
         <v>8</v>
@@ -2914,12 +2909,12 @@
         <v>8</v>
       </c>
       <c r="S34" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>
       <c r="V34" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W34" s="4">
         <v>8</v>
@@ -2931,7 +2926,7 @@
         <v>8</v>
       </c>
       <c r="Z34" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA34" s="7"/>
       <c r="AB34" s="7"/>
@@ -2946,48 +2941,48 @@
         <v>8</v>
       </c>
       <c r="AG34" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH34" s="7"/>
       <c r="AI34" s="7"/>
       <c r="AJ34" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK34" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL34" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="2:38" ht="15" customHeight="1">
+    <row r="35" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>14</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E35" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="10">
         <v>9</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L35" s="4">
         <v>8</v>
@@ -3001,38 +2996,38 @@
         <v>8</v>
       </c>
       <c r="Q35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
       <c r="V35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA35" s="7"/>
       <c r="AB35" s="7"/>
       <c r="AC35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD35" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE35" s="5"/>
       <c r="AF35" s="4">
@@ -3044,49 +3039,49 @@
       <c r="AH35" s="7"/>
       <c r="AI35" s="7"/>
       <c r="AJ35" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK35" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AL35" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="36" spans="2:38" ht="15" customHeight="1">
+    <row r="36" spans="2:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>19</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E36" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>54</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P36" s="4">
         <v>8</v>
@@ -3095,18 +3090,18 @@
         <v>8</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="T36" s="7"/>
       <c r="U36" s="7"/>
       <c r="V36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="W36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="X36" s="4">
         <v>8</v>
@@ -3115,7 +3110,7 @@
         <v>8</v>
       </c>
       <c r="Z36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AA36" s="7"/>
       <c r="AB36" s="7"/>
@@ -3127,15 +3122,15 @@
       </c>
       <c r="AE36" s="5"/>
       <c r="AF36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AG36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AH36" s="7"/>
       <c r="AI36" s="7"/>
       <c r="AJ36" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AK36" s="4">
         <v>8</v>
@@ -3170,1013 +3165,1013 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1" x14ac:dyDescent="0.25"/>
+    <row r="2" x14ac:dyDescent="0.25"/>
+    <row r="3" x14ac:dyDescent="0.25"/>
+    <row r="4" x14ac:dyDescent="0.25"/>
+    <row r="5" x14ac:dyDescent="0.25"/>
+    <row r="6" x14ac:dyDescent="0.25"/>
+    <row r="7" x14ac:dyDescent="0.25"/>
+    <row r="8" x14ac:dyDescent="0.25"/>
+    <row r="9" x14ac:dyDescent="0.25"/>
+    <row r="10" x14ac:dyDescent="0.25"/>
+    <row r="11" x14ac:dyDescent="0.25"/>
+    <row r="12" x14ac:dyDescent="0.25"/>
+    <row r="13" x14ac:dyDescent="0.25"/>
+    <row r="14" x14ac:dyDescent="0.25"/>
+    <row r="15" x14ac:dyDescent="0.25"/>
+    <row r="16" x14ac:dyDescent="0.25"/>
+    <row r="17" x14ac:dyDescent="0.25"/>
+    <row r="18" x14ac:dyDescent="0.25"/>
+    <row r="19" x14ac:dyDescent="0.25"/>
+    <row r="20" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4194,6 +4189,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080ACE09E7D8F4A4D99A534D3EB20B34C" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="18b97ffed73d5344a6e767d655bb596d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c720f9d8-444b-4fbe-babb-a5ce851220a8" xmlns:ns3="b8cacd15-12fa-49cc-bc89-63acc881fe72" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3e13d56453452055be885cd81c70138" ns2:_="" ns3:_="">
     <xsd:import namespace="c720f9d8-444b-4fbe-babb-a5ce851220a8"/>
@@ -4370,20 +4371,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01348843-B7B5-44F8-89A1-8FBD6D46374E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01348843-B7B5-44F8-89A1-8FBD6D46374E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDABD5D4-B5D1-4A95-BCE9-7CF20D1138A5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{394E89AC-A862-46CE-901C-2082B988E1EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{394E89AC-A862-46CE-901C-2082B988E1EA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDABD5D4-B5D1-4A95-BCE9-7CF20D1138A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c720f9d8-444b-4fbe-babb-a5ce851220a8"/>
+    <ds:schemaRef ds:uri="b8cacd15-12fa-49cc-bc89-63acc881fe72"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>